<commit_message>
Updated DOES>, COMPILE, and RECURSE to use the JSL instruction rather than JSR IS and DEFER to be considered
</commit_message>
<xml_diff>
--- a/Resources/Benchmarks.xlsx
+++ b/Resources/Benchmarks.xlsx
@@ -492,7 +492,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -785,15 +785,15 @@
         <v>44272</v>
       </c>
       <c r="E17" s="3">
-        <v>40477</v>
+        <v>37947</v>
       </c>
       <c r="F17" s="13">
         <f t="shared" si="1"/>
-        <v>1.0937569483904439</v>
+        <v>1.1666798429388356</v>
       </c>
       <c r="G17" s="9">
         <f t="shared" ref="G17:G21" si="2">E17/C17</f>
-        <v>144.04626334519574</v>
+        <v>135.04270462633451</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -906,15 +906,15 @@
       </c>
       <c r="E22" s="7">
         <f>SUM(E16:E21)</f>
-        <v>174442</v>
+        <v>171912</v>
       </c>
       <c r="F22" s="13">
         <f t="shared" si="1"/>
-        <v>1.1610391992754039</v>
+        <v>1.1781260179626787</v>
       </c>
       <c r="G22" s="10">
         <f>E22/C22</f>
-        <v>166.77055449330783</v>
+        <v>164.35181644359466</v>
       </c>
     </row>
     <row r="23" spans="1:7">

</xml_diff>

<commit_message>
Replaced JSR with JSL in SRAM.asm
</commit_message>
<xml_diff>
--- a/Resources/Benchmarks.xlsx
+++ b/Resources/Benchmarks.xlsx
@@ -87,7 +87,7 @@
     <t>NIGE 1.1 / 1.0</t>
   </si>
   <si>
-    <t>NIGE 1.1/VFX</t>
+    <t>NIGE 1.1 / VFX</t>
   </si>
 </sst>
 </file>
@@ -135,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -150,15 +150,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -192,7 +183,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -492,7 +483,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -501,7 +492,7 @@
     <col min="2" max="2" width="16.5703125" style="4" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" style="4" customWidth="1"/>
     <col min="4" max="6" width="18.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -590,7 +581,7 @@
         <v>260</v>
       </c>
       <c r="F7" s="13">
-        <f>D7/E7</f>
+        <f>E7/D7</f>
         <v>1</v>
       </c>
     </row>
@@ -611,8 +602,8 @@
         <v>300</v>
       </c>
       <c r="F8" s="13">
-        <f t="shared" ref="F8:F13" si="0">D8/E8</f>
-        <v>1.1333333333333333</v>
+        <f t="shared" ref="F8:F14" si="0">E8/D8</f>
+        <v>0.88235294117647056</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -633,7 +624,7 @@
       </c>
       <c r="F9" s="13">
         <f t="shared" si="0"/>
-        <v>1.0476190476190477</v>
+        <v>0.95454545454545459</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -654,7 +645,7 @@
       </c>
       <c r="F10" s="13">
         <f t="shared" si="0"/>
-        <v>1.0333333333333334</v>
+        <v>0.967741935483871</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -675,7 +666,7 @@
       </c>
       <c r="F11" s="13">
         <f t="shared" si="0"/>
-        <v>1.0333333333333334</v>
+        <v>0.967741935483871</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -696,7 +687,7 @@
       </c>
       <c r="F12" s="13">
         <f t="shared" si="0"/>
-        <v>1.0142857142857142</v>
+        <v>0.9859154929577465</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -713,11 +704,11 @@
         <v>9008</v>
       </c>
       <c r="E13" s="3">
-        <v>7407</v>
-      </c>
-      <c r="F13" s="14">
+        <v>7207</v>
+      </c>
+      <c r="F13" s="13">
         <f t="shared" si="0"/>
-        <v>1.2161468880788444</v>
+        <v>0.80006660746003555</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -730,11 +721,11 @@
       </c>
       <c r="E14" s="7">
         <f>SUM(E7:E13)</f>
-        <v>12187</v>
-      </c>
-      <c r="F14" s="13">
-        <f t="shared" ref="F14:F22" si="1">D14/E14</f>
-        <v>1.1444982358250595</v>
+        <v>11987</v>
+      </c>
+      <c r="F14" s="14">
+        <f t="shared" si="0"/>
+        <v>0.85940636650415825</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -763,8 +754,8 @@
         <v>18884</v>
       </c>
       <c r="F16" s="13">
-        <f t="shared" si="1"/>
-        <v>1.0421520864223681</v>
+        <f t="shared" ref="F16:F22" si="1">E16/D16</f>
+        <v>0.95955284552845532</v>
       </c>
       <c r="G16" s="9">
         <f>E16/C16</f>
@@ -776,7 +767,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="5">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="C17" s="5">
         <v>281</v>
@@ -789,7 +780,7 @@
       </c>
       <c r="F17" s="13">
         <f t="shared" si="1"/>
-        <v>1.1666798429388356</v>
+        <v>0.85713317672569567</v>
       </c>
       <c r="G17" s="9">
         <f t="shared" ref="G17:G21" si="2">E17/C17</f>
@@ -810,15 +801,15 @@
         <v>10924</v>
       </c>
       <c r="E18" s="3">
-        <v>9550</v>
+        <v>9410</v>
       </c>
       <c r="F18" s="13">
         <f t="shared" si="1"/>
-        <v>1.1438743455497382</v>
+        <v>0.86140607835957528</v>
       </c>
       <c r="G18" s="9">
         <f t="shared" si="2"/>
-        <v>308.06451612903226</v>
+        <v>303.54838709677421</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -835,15 +826,15 @@
         <v>48795</v>
       </c>
       <c r="E19" s="3">
-        <v>36319</v>
+        <v>35643</v>
       </c>
       <c r="F19" s="13">
         <f t="shared" si="1"/>
-        <v>1.3435116605633415</v>
+        <v>0.73046418690439596</v>
       </c>
       <c r="G19" s="9">
         <f t="shared" si="2"/>
-        <v>129.2491103202847</v>
+        <v>126.84341637010677</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -860,15 +851,15 @@
         <v>41089</v>
       </c>
       <c r="E20" s="3">
-        <v>33389</v>
+        <v>33387</v>
       </c>
       <c r="F20" s="13">
         <f t="shared" si="1"/>
-        <v>1.2306148731618198</v>
+        <v>0.81255323809292024</v>
       </c>
       <c r="G20" s="9">
         <f t="shared" si="2"/>
-        <v>153.16055045871559</v>
+        <v>153.151376146789</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -885,15 +876,15 @@
         <v>37774</v>
       </c>
       <c r="E21" s="3">
-        <v>35823</v>
-      </c>
-      <c r="F21" s="14">
+        <v>26968</v>
+      </c>
+      <c r="F21" s="13">
         <f t="shared" si="1"/>
-        <v>1.0544622170114173</v>
+        <v>0.71393021655106692</v>
       </c>
       <c r="G21" s="9">
         <f t="shared" si="2"/>
-        <v>254.06382978723406</v>
+        <v>191.26241134751774</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -906,15 +897,15 @@
       </c>
       <c r="E22" s="7">
         <f>SUM(E16:E21)</f>
-        <v>171912</v>
-      </c>
-      <c r="F22" s="13">
+        <v>162239</v>
+      </c>
+      <c r="F22" s="14">
         <f t="shared" si="1"/>
-        <v>1.1781260179626787</v>
+        <v>0.80104575034315229</v>
       </c>
       <c r="G22" s="10">
         <f>E22/C22</f>
-        <v>164.35181644359466</v>
+        <v>155.10420650095602</v>
       </c>
     </row>
     <row r="23" spans="1:7">

</xml_diff>

<commit_message>
Initial benchmarking of NIGE 2.0
</commit_message>
<xml_diff>
--- a/Resources/Benchmarks.xlsx
+++ b/Resources/Benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="19155" windowHeight="10800" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="19155" windowHeight="10800"/>
   </bookViews>
   <sheets>
     <sheet name="perfomance" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="96">
   <si>
     <t>DO LOOP</t>
   </si>
@@ -298,6 +298,12 @@
   </si>
   <si>
     <t>6438 bytes free</t>
+  </si>
+  <si>
+    <t>NIGE 2.0</t>
+  </si>
+  <si>
+    <t>NIGE 2.0 / 1.0</t>
   </si>
 </sst>
 </file>
@@ -709,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -722,13 +728,14 @@
     <col min="3" max="3" width="18.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23" style="1" customWidth="1"/>
-    <col min="7" max="8" width="18.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="7" width="23" style="1" customWidth="1"/>
+    <col min="8" max="9" width="18.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="C1" s="8" t="s">
         <v>16</v>
       </c>
@@ -742,24 +749,31 @@
         <v>90</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="K1" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -771,21 +785,15 @@
         <v>8064</v>
       </c>
       <c r="D3" s="3">
-        <f>508+409+937+1011+1008</f>
-        <v>3873</v>
-      </c>
-      <c r="E3" s="3">
-        <f>508+409+937+1048+1008</f>
-        <v>3910</v>
-      </c>
-      <c r="F3" s="3">
-        <f>508+409+937+1048+1008</f>
-        <v>3910</v>
-      </c>
+        <v>4742</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="I3" s="3"/>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -802,10 +810,13 @@
         <v>19</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -824,16 +835,23 @@
       <c r="F6" s="3">
         <v>260</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="3">
+        <v>240</v>
+      </c>
+      <c r="H6" s="13">
         <f>E6/D6</f>
         <v>1</v>
       </c>
-      <c r="H6" s="13">
+      <c r="I6" s="13">
         <f>E6/F6</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="K6" s="13">
+        <f>G6/D6</f>
+        <v>0.92307692307692313</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -852,16 +870,23 @@
       <c r="F7" s="3">
         <v>300</v>
       </c>
-      <c r="G7" s="13">
-        <f t="shared" ref="G7:G13" si="0">E7/D7</f>
+      <c r="G7" s="3">
+        <v>300</v>
+      </c>
+      <c r="H7" s="13">
+        <f t="shared" ref="H7:H13" si="0">E7/D7</f>
         <v>0.88235294117647056</v>
       </c>
-      <c r="H7" s="13">
-        <f t="shared" ref="H7:H21" si="1">E7/F7</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="I7" s="13">
+        <f t="shared" ref="I7:I21" si="1">E7/F7</f>
+        <v>1</v>
+      </c>
+      <c r="K7" s="13">
+        <f t="shared" ref="K7:K21" si="2">G7/D7</f>
+        <v>0.88235294117647056</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -880,16 +905,23 @@
       <c r="F8" s="3">
         <v>420</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="3">
+        <v>400</v>
+      </c>
+      <c r="H8" s="13">
         <f t="shared" si="0"/>
         <v>0.95454545454545459</v>
       </c>
-      <c r="H8" s="13">
+      <c r="I8" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="K8" s="13">
+        <f t="shared" si="2"/>
+        <v>0.90909090909090906</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -908,16 +940,23 @@
       <c r="F9" s="3">
         <v>1200</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="3">
+        <v>1200</v>
+      </c>
+      <c r="H9" s="13">
         <f t="shared" si="0"/>
         <v>0.967741935483871</v>
       </c>
-      <c r="H9" s="13">
+      <c r="I9" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="K9" s="13">
+        <f t="shared" si="2"/>
+        <v>0.967741935483871</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -936,16 +975,23 @@
       <c r="F10" s="3">
         <v>1200</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="3">
+        <v>1200</v>
+      </c>
+      <c r="H10" s="13">
         <f t="shared" si="0"/>
         <v>0.967741935483871</v>
       </c>
-      <c r="H10" s="13">
+      <c r="I10" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="K10" s="13">
+        <f t="shared" si="2"/>
+        <v>0.967741935483871</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -964,16 +1010,23 @@
       <c r="F11" s="3">
         <v>1400</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="3">
+        <v>1380</v>
+      </c>
+      <c r="H11" s="13">
         <f t="shared" si="0"/>
         <v>0.9859154929577465</v>
       </c>
-      <c r="H11" s="13">
+      <c r="I11" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="K11" s="13">
+        <f t="shared" si="2"/>
+        <v>0.971830985915493</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -992,16 +1045,23 @@
       <c r="F12" s="3">
         <v>7207</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="3">
+        <v>7006</v>
+      </c>
+      <c r="H12" s="13">
         <f t="shared" si="0"/>
         <v>0.80006660746003555</v>
       </c>
-      <c r="H12" s="13">
+      <c r="I12" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="K12" s="13">
+        <f t="shared" si="2"/>
+        <v>0.77775310834813494</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="C13" s="6">
         <v>31</v>
       </c>
@@ -1017,16 +1077,23 @@
         <f>SUM(F6:F12)</f>
         <v>11987</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="7">
+        <v>11726</v>
+      </c>
+      <c r="H13" s="14">
         <f t="shared" si="0"/>
         <v>0.85940636650415825</v>
       </c>
-      <c r="H13" s="14">
+      <c r="I13" s="14">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="K13" s="14">
+        <f t="shared" si="2"/>
+        <v>0.84069400630914826</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -1036,8 +1103,10 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="I14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -1056,20 +1125,27 @@
       <c r="F15" s="3">
         <v>18884</v>
       </c>
-      <c r="G15" s="13">
-        <f t="shared" ref="G15:G21" si="2">E15/D15</f>
+      <c r="G15" s="3">
+        <v>18454</v>
+      </c>
+      <c r="H15" s="13">
+        <f t="shared" ref="H15:H21" si="3">E15/D15</f>
         <v>0.95955284552845532</v>
       </c>
-      <c r="H15" s="13">
+      <c r="I15" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I15" s="9">
+      <c r="J15" s="9">
         <f>E15/C15</f>
         <v>171.67272727272729</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="K15" s="13">
+        <f t="shared" si="2"/>
+        <v>0.93770325203252036</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -1088,20 +1164,27 @@
       <c r="F16" s="3">
         <v>37947</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="3">
+        <v>34152</v>
+      </c>
+      <c r="H16" s="13">
+        <f t="shared" si="3"/>
+        <v>0.85713317672569567</v>
+      </c>
+      <c r="I16" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J16" s="9">
+        <f t="shared" ref="J16:J20" si="4">E16/C16</f>
+        <v>143.19622641509434</v>
+      </c>
+      <c r="K16" s="13">
         <f t="shared" si="2"/>
-        <v>0.85713317672569567</v>
-      </c>
-      <c r="H16" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I16" s="9">
-        <f t="shared" ref="I16:I20" si="3">E16/C16</f>
-        <v>143.19622641509434</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>0.77141308276111309</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1120,20 +1203,27 @@
       <c r="F17" s="3">
         <v>9410</v>
       </c>
-      <c r="G17" s="13">
-        <f t="shared" si="2"/>
+      <c r="G17" s="3">
+        <v>12840</v>
+      </c>
+      <c r="H17" s="13">
+        <f t="shared" si="3"/>
         <v>0.83952764555108017</v>
       </c>
-      <c r="H17" s="13">
+      <c r="I17" s="13">
         <f t="shared" si="1"/>
         <v>0.97460148777895861</v>
       </c>
-      <c r="I17" s="9">
-        <f t="shared" si="3"/>
+      <c r="J17" s="9">
+        <f t="shared" si="4"/>
         <v>295.83870967741933</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="K17" s="13">
+        <f t="shared" si="2"/>
+        <v>1.1753936287074331</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
@@ -1152,20 +1242,27 @@
       <c r="F18" s="3">
         <v>35643</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="3">
+        <v>36970</v>
+      </c>
+      <c r="H18" s="13">
+        <f t="shared" si="3"/>
+        <v>0.73046418690439596</v>
+      </c>
+      <c r="I18" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J18" s="9">
+        <f t="shared" si="4"/>
+        <v>120.41554054054055</v>
+      </c>
+      <c r="K18" s="13">
         <f t="shared" si="2"/>
-        <v>0.73046418690439596</v>
-      </c>
-      <c r="H18" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I18" s="9">
-        <f t="shared" si="3"/>
-        <v>120.41554054054055</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>0.75765959627010959</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -1184,20 +1281,27 @@
       <c r="F19" s="3">
         <v>33387</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="3">
+        <v>34669</v>
+      </c>
+      <c r="H19" s="13">
+        <f t="shared" si="3"/>
+        <v>0.81255323809292024</v>
+      </c>
+      <c r="I19" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J19" s="9">
+        <f t="shared" si="4"/>
+        <v>153.151376146789</v>
+      </c>
+      <c r="K19" s="13">
         <f t="shared" si="2"/>
-        <v>0.81255323809292024</v>
-      </c>
-      <c r="H19" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I19" s="9">
-        <f t="shared" si="3"/>
-        <v>153.151376146789</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>0.84375380272092293</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
@@ -1216,20 +1320,27 @@
       <c r="F20" s="3">
         <v>26968</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="3">
+        <v>24000</v>
+      </c>
+      <c r="H20" s="13">
+        <f t="shared" si="3"/>
+        <v>0.71393021655106692</v>
+      </c>
+      <c r="I20" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J20" s="9">
+        <f t="shared" si="4"/>
+        <v>191.26241134751774</v>
+      </c>
+      <c r="K20" s="13">
         <f t="shared" si="2"/>
-        <v>0.71393021655106692</v>
-      </c>
-      <c r="H20" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I20" s="9">
-        <f t="shared" si="3"/>
-        <v>191.26241134751774</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>0.63535765341240003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="C21" s="6">
         <v>1046</v>
       </c>
@@ -1245,28 +1356,37 @@
         <f>SUM(F15:F20)</f>
         <v>162239</v>
       </c>
-      <c r="G21" s="14">
-        <f t="shared" si="2"/>
+      <c r="G21" s="7">
+        <v>161085</v>
+      </c>
+      <c r="H21" s="14">
+        <f t="shared" si="3"/>
         <v>0.79986570156121939</v>
       </c>
-      <c r="H21" s="14">
+      <c r="I21" s="14">
         <f t="shared" si="1"/>
         <v>0.99852686468728236</v>
       </c>
-      <c r="I21" s="10">
+      <c r="J21" s="10">
         <f>E21/C21</f>
         <v>154.87571701720842</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="K21" s="14">
+        <f t="shared" si="2"/>
+        <v>0.79534794158017919</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="C22" s="12"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="I22" s="11"/>
+      <c r="K22" s="13"/>
+    </row>
+    <row r="24" spans="1:11">
       <c r="E24" s="1" t="s">
         <v>93</v>
       </c>
@@ -1284,7 +1404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Corrected V1.0 benchmark for error in D+ Updated cursor handling in screen control
</commit_message>
<xml_diff>
--- a/Resources/Benchmarks.xlsx
+++ b/Resources/Benchmarks.xlsx
@@ -15,6 +15,30 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Andrew</author>
+  </authors>
+  <commentList>
+    <comment ref="E17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Faulty D+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="96">
   <si>
@@ -315,7 +339,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,6 +364,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -386,7 +423,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -416,6 +453,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -718,7 +756,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -789,7 +827,9 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="G3" s="3">
+        <v>4779</v>
+      </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
@@ -1195,12 +1235,12 @@
         <v>31</v>
       </c>
       <c r="D17" s="3">
-        <v>10924</v>
-      </c>
-      <c r="E17" s="3">
+        <v>15831</v>
+      </c>
+      <c r="E17" s="17">
         <v>9171</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="17">
         <v>9410</v>
       </c>
       <c r="G17" s="3">
@@ -1208,7 +1248,7 @@
       </c>
       <c r="H17" s="13">
         <f t="shared" si="3"/>
-        <v>0.83952764555108017</v>
+        <v>0.57930642410460487</v>
       </c>
       <c r="I17" s="13">
         <f t="shared" si="1"/>
@@ -1220,7 +1260,7 @@
       </c>
       <c r="K17" s="13">
         <f t="shared" si="2"/>
-        <v>1.1753936287074331</v>
+        <v>0.81106689406859955</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1346,7 +1386,7 @@
       </c>
       <c r="D21" s="7">
         <f>SUM(D15:D20)</f>
-        <v>202534</v>
+        <v>207441</v>
       </c>
       <c r="E21" s="7">
         <f>SUM(E15:E20)</f>
@@ -1361,7 +1401,7 @@
       </c>
       <c r="H21" s="14">
         <f t="shared" si="3"/>
-        <v>0.79986570156121939</v>
+        <v>0.78094494338149156</v>
       </c>
       <c r="I21" s="14">
         <f t="shared" si="1"/>
@@ -1373,7 +1413,7 @@
       </c>
       <c r="K21" s="14">
         <f t="shared" si="2"/>
-        <v>0.79534794158017919</v>
+        <v>0.77653405064572578</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1397,6 +1437,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1423,10 +1464,10 @@
       <c r="B1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="17"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:5">
       <c r="D2" s="4" t="s">

</xml_diff>